<commit_message>
Revised tests to include Chrome/IE specific ones
</commit_message>
<xml_diff>
--- a/tests/revival-records-testing-admin-content-editing.xlsx
+++ b/tests/revival-records-testing-admin-content-editing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t>PASSED</t>
   </si>
@@ -42,36 +42,24 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>Testing admin home editing functionality</t>
-  </si>
-  <si>
     <t>From home page, I click on admin login</t>
   </si>
   <si>
     <t>You are required to login</t>
   </si>
   <si>
-    <t>Open site in browser (Chrome, IE)</t>
-  </si>
-  <si>
     <t>I click on the link to edit home</t>
   </si>
   <si>
     <t>Content and title inputs are shown in three columns</t>
   </si>
   <si>
-    <t>Change text for one content area</t>
-  </si>
-  <si>
     <t>Click submit changes</t>
   </si>
   <si>
     <t>Page reloads, displays confirmation success</t>
   </si>
   <si>
-    <t>Testing admin contact editing functionality</t>
-  </si>
-  <si>
     <t>Page loads and shows buttons to four areas</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t>Content inputs are shown in two columns</t>
   </si>
   <si>
-    <t>Testing admin about editing functionality</t>
-  </si>
-  <si>
     <t>I click on the link to edit contact</t>
   </si>
   <si>
@@ -103,6 +88,39 @@
   </si>
   <si>
     <t>Content is changed</t>
+  </si>
+  <si>
+    <t>Testing admin home editing functionality in Chrome</t>
+  </si>
+  <si>
+    <t>Open site in browser in IE</t>
+  </si>
+  <si>
+    <t>Open site in browser in Chrome</t>
+  </si>
+  <si>
+    <t>Testing admin about editing functionality in IE</t>
+  </si>
+  <si>
+    <t>Testing admin home editing functionality in IE</t>
+  </si>
+  <si>
+    <t>Testing admin contact editing functionality in Chrome</t>
+  </si>
+  <si>
+    <t>From home page, I click on admin login (footer)</t>
+  </si>
+  <si>
+    <t>Change text for 1, 2, or 3 content areas</t>
+  </si>
+  <si>
+    <t>Testing admin about editing functionality in Chrome</t>
+  </si>
+  <si>
+    <t>Change text for 1 or 2 content areas</t>
+  </si>
+  <si>
+    <t>Testing admin contact editing functionality in IE</t>
   </si>
 </sst>
 </file>
@@ -809,9 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -845,10 +865,10 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -858,10 +878,10 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
       <c r="B3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -871,7 +891,7 @@
       <c r="A4" s="36"/>
       <c r="B4" s="14"/>
       <c r="C4" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -880,7 +900,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>5</v>
@@ -893,7 +913,7 @@
       <c r="A6" s="36"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -902,10 +922,10 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="B7" s="14" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -914,10 +934,10 @@
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -927,7 +947,7 @@
       <c r="A9" s="36"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -937,52 +957,52 @@
       <c r="A10" s="37"/>
       <c r="B10" s="16"/>
       <c r="C10" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="19"/>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="13"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>9</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22" t="s">
-        <v>17</v>
+      <c r="A13" s="36"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="21"/>
@@ -990,54 +1010,54 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22" t="s">
-        <v>22</v>
+      <c r="A15" s="36"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>18</v>
+      <c r="A16" s="36"/>
+      <c r="B16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>15</v>
+      <c r="A17" s="36"/>
+      <c r="B17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22" t="s">
-        <v>20</v>
+      <c r="A18" s="36"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24" t="s">
-        <v>19</v>
+      <c r="A19" s="37"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -1045,10 +1065,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="27"/>
@@ -1058,10 +1078,10 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>9</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -1071,7 +1091,7 @@
       <c r="A22" s="36"/>
       <c r="B22" s="14"/>
       <c r="C22" s="15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -1080,7 +1100,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="36"/>
       <c r="B23" s="14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>5</v>
@@ -1093,7 +1113,7 @@
       <c r="A24" s="36"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -1102,22 +1122,22 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="36"/>
       <c r="B26" s="14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -1127,7 +1147,7 @@
       <c r="A27" s="36"/>
       <c r="B27" s="14"/>
       <c r="C27" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -1137,87 +1157,119 @@
       <c r="A28" s="37"/>
       <c r="B28" s="16"/>
       <c r="C28" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="31"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="19"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
+    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="39"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22" t="s">
+        <v>13</v>
+      </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="36"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>14</v>
+      </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
+    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="39"/>
+      <c r="B35" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
+    <row r="37" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="40"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24" t="s">
+        <v>15</v>
+      </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
       <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>25</v>
+      </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
@@ -1225,88 +1277,122 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="36"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="36"/>
       <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="36"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="15"/>
+      <c r="B41" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
       <c r="B42" s="14"/>
-      <c r="C42" s="15"/>
+      <c r="C42" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="36"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="36"/>
       <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
+      <c r="C45" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="31"/>
+    <row r="46" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="37"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="31"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="11"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="33"/>
+      <c r="B48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="5"/>
@@ -1314,74 +1400,90 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="33"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="7"/>
+      <c r="C51" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="33"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="7"/>
+      <c r="B52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="33"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="7"/>
+      <c r="B53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="33"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="33"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="5"/>
+    <row r="55" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="34"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="31"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="33"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="34"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="31"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="33"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="33"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="11"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="33"/>
@@ -1431,37 +1533,37 @@
       <c r="E64" s="6"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="33"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="5"/>
+    <row r="65" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="34"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="31"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="33"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="34"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="31"/>
+      <c r="A66" s="32"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="11"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="33"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="11"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="33"/>
@@ -1511,40 +1613,24 @@
       <c r="E74" s="6"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="33"/>
-      <c r="B75" s="6"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="33"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="34"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="31"/>
+    <row r="75" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="34"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="A58:A67"/>
-    <mergeCell ref="A68:A77"/>
+    <mergeCell ref="A47:A55"/>
+    <mergeCell ref="A56:A65"/>
+    <mergeCell ref="A66:A75"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A19"/>
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="A29:A37"/>
-    <mergeCell ref="A38:A47"/>
+    <mergeCell ref="A38:A46"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>